<commit_message>
upload latest def file
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v05_collection_view.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v05_collection_view.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/Documents/Definition Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825EB1CE-FA91-2E4C-B901-754313063870}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC502104-5E47-F140-B3A0-1FEFAC91C9F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="460" windowWidth="28800" windowHeight="16100" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30820" yWindow="4320" windowWidth="28800" windowHeight="16440" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="484">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1560,19 +1560,19 @@
     <t>auto.ccd.fe@gmail.com</t>
   </si>
   <si>
+    <t>CollectionComplexField</t>
+  </si>
+  <si>
+    <t>Collection of Complex</t>
+  </si>
+  <si>
+    <t>#TABLE(AddressLine1)</t>
+  </si>
+  <si>
+    <t>#TABLE(AddressLine1, AddressLine1, AddressLine1,Country)</t>
+  </si>
+  <si>
     <t>DisplayContextParameter</t>
-  </si>
-  <si>
-    <t>CollectionComplexField</t>
-  </si>
-  <si>
-    <t>#TABLE(AddressLine1, AddressLine1, AddressLine1,Country)</t>
-  </si>
-  <si>
-    <t>Collection of Complex</t>
-  </si>
-  <si>
-    <t>#TABLE(AddressLine1)</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1583,7 @@
     <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
     <numFmt numFmtId="165" formatCode="&quot;D/&quot;m&quot;/YY&quot;"/>
   </numFmts>
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1842,25 +1842,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF032F62"/>
       <name val="Consolas"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1930,6 +1918,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2030,7 +2024,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2181,9 +2175,18 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="13" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="26" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="13" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="26" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -3530,10 +3533,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AC44"/>
+  <dimension ref="A1:AD44"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView showGridLines="0" topLeftCell="H2" workbookViewId="0">
+      <selection activeCell="N2" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3549,14 +3552,14 @@
     <col min="9" max="9" width="40" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="17.83203125" style="22" customWidth="1"/>
     <col min="12" max="13" width="22" style="22" customWidth="1"/>
-    <col min="14" max="14" width="22" style="42" customWidth="1"/>
+    <col min="14" max="14" width="22" style="145" customWidth="1"/>
     <col min="15" max="15" width="42.5" style="22" customWidth="1"/>
     <col min="16" max="16" width="28.33203125" style="22" customWidth="1"/>
     <col min="17" max="29" width="8.83203125" style="22" customWidth="1"/>
     <col min="30" max="257" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>196</v>
       </c>
@@ -3578,7 +3581,7 @@
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="N1" s="142"/>
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
@@ -3595,7 +3598,7 @@
       <c r="AB1" s="7"/>
       <c r="AC1" s="7"/>
     </row>
-    <row r="2" spans="1:29" ht="68.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" ht="68.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -3635,7 +3638,7 @@
       <c r="M2" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="N2" s="8"/>
+      <c r="N2" s="137"/>
       <c r="O2" s="9" t="s">
         <v>207</v>
       </c>
@@ -3656,7 +3659,7 @@
       <c r="AB2" s="6"/>
       <c r="AC2" s="6"/>
     </row>
-    <row r="3" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -3696,8 +3699,8 @@
       <c r="M3" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="N3" s="136" t="s">
-        <v>479</v>
+      <c r="N3" s="138" t="s">
+        <v>483</v>
       </c>
       <c r="O3" s="8" t="s">
         <v>216</v>
@@ -3719,7 +3722,7 @@
       <c r="AB3" s="7"/>
       <c r="AC3" s="7"/>
     </row>
-    <row r="4" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42736</v>
       </c>
@@ -3751,7 +3754,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
+      <c r="N4" s="142"/>
       <c r="O4" s="8" t="s">
         <v>195</v>
       </c>
@@ -3770,7 +3773,7 @@
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
     </row>
-    <row r="5" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42736</v>
       </c>
@@ -3802,7 +3805,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="N5" s="142"/>
       <c r="O5" s="8" t="s">
         <v>195</v>
       </c>
@@ -3821,7 +3824,7 @@
       <c r="AB5" s="7"/>
       <c r="AC5" s="7"/>
     </row>
-    <row r="6" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42736</v>
       </c>
@@ -3853,7 +3856,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="N6" s="142"/>
       <c r="O6" s="8" t="s">
         <v>195</v>
       </c>
@@ -3872,7 +3875,7 @@
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
     </row>
-    <row r="7" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42736</v>
       </c>
@@ -3904,7 +3907,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
+      <c r="N7" s="142"/>
       <c r="O7" s="8" t="s">
         <v>195</v>
       </c>
@@ -3923,7 +3926,7 @@
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
     </row>
-    <row r="8" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42736</v>
       </c>
@@ -3955,7 +3958,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="N8" s="142"/>
       <c r="O8" s="8" t="s">
         <v>195</v>
       </c>
@@ -3974,7 +3977,7 @@
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
     </row>
-    <row r="9" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>42736</v>
       </c>
@@ -4006,7 +4009,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="N9" s="142"/>
       <c r="O9" s="8" t="s">
         <v>195</v>
       </c>
@@ -4025,7 +4028,7 @@
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
     </row>
-    <row r="10" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>42736</v>
       </c>
@@ -4057,7 +4060,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
+      <c r="N10" s="142"/>
       <c r="O10" s="8" t="s">
         <v>195</v>
       </c>
@@ -4076,7 +4079,7 @@
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
     </row>
-    <row r="11" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10">
         <v>42736</v>
       </c>
@@ -4108,7 +4111,7 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="138"/>
+      <c r="N11" s="142"/>
       <c r="O11" s="8" t="s">
         <v>195</v>
       </c>
@@ -4127,60 +4130,60 @@
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
     </row>
-    <row r="12" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="8" t="s">
+    <row r="12" spans="1:30" s="144" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="136">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="136"/>
+      <c r="C12" s="137" t="s">
         <v>397</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="137" t="s">
         <v>193</v>
       </c>
-      <c r="E12" s="57" t="s">
-        <v>480</v>
-      </c>
-      <c r="F12" s="23">
+      <c r="E12" s="138" t="s">
+        <v>479</v>
+      </c>
+      <c r="F12" s="146">
         <v>1</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="137" t="s">
         <v>218</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="137" t="s">
         <v>219</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="137" t="s">
         <v>220</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="141">
         <v>1</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="138" t="s">
-        <v>481</v>
-      </c>
-      <c r="O12" s="8" t="s">
+      <c r="K12" s="142"/>
+      <c r="L12" s="142"/>
+      <c r="M12" s="142"/>
+      <c r="N12" s="143" t="s">
+        <v>482</v>
+      </c>
+      <c r="O12" s="137" t="s">
         <v>195</v>
       </c>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="7"/>
-    </row>
-    <row r="13" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q12" s="142"/>
+      <c r="R12" s="142"/>
+      <c r="S12" s="142"/>
+      <c r="T12" s="142"/>
+      <c r="U12" s="142"/>
+      <c r="V12" s="142"/>
+      <c r="W12" s="142"/>
+      <c r="X12" s="142"/>
+      <c r="Y12" s="142"/>
+      <c r="Z12" s="142"/>
+      <c r="AA12" s="142"/>
+      <c r="AB12" s="142"/>
+      <c r="AC12" s="142"/>
+      <c r="AD12" s="142"/>
+    </row>
+    <row r="13" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10">
         <v>42736</v>
       </c>
@@ -4212,7 +4215,7 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
+      <c r="N13" s="142"/>
       <c r="O13" s="8" t="s">
         <v>195</v>
       </c>
@@ -4231,7 +4234,7 @@
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
     </row>
-    <row r="14" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10">
         <v>42736</v>
       </c>
@@ -4263,7 +4266,7 @@
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
+      <c r="N14" s="142"/>
       <c r="O14" s="8" t="s">
         <v>195</v>
       </c>
@@ -4282,7 +4285,7 @@
       <c r="AB14" s="7"/>
       <c r="AC14" s="7"/>
     </row>
-    <row r="15" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10">
         <v>42736</v>
       </c>
@@ -4314,7 +4317,7 @@
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
+      <c r="N15" s="142"/>
       <c r="O15" s="8" t="s">
         <v>195</v>
       </c>
@@ -4333,7 +4336,7 @@
       <c r="AB15" s="7"/>
       <c r="AC15" s="7"/>
     </row>
-    <row r="16" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:30" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10">
         <v>42736</v>
       </c>
@@ -4365,7 +4368,7 @@
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
+      <c r="N16" s="142"/>
       <c r="O16" s="8" t="s">
         <v>195</v>
       </c>
@@ -4416,7 +4419,7 @@
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
+      <c r="N17" s="142"/>
       <c r="O17" s="8" t="s">
         <v>195</v>
       </c>
@@ -4467,7 +4470,7 @@
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
+      <c r="N18" s="142"/>
       <c r="O18" s="8" t="s">
         <v>195</v>
       </c>
@@ -4518,7 +4521,7 @@
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
+      <c r="N19" s="142"/>
       <c r="O19" s="8" t="s">
         <v>195</v>
       </c>
@@ -4569,7 +4572,7 @@
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
+      <c r="N20" s="142"/>
       <c r="O20" s="8" t="s">
         <v>195</v>
       </c>
@@ -4620,7 +4623,7 @@
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
+      <c r="N21" s="142"/>
       <c r="O21" s="8" t="s">
         <v>195</v>
       </c>
@@ -4671,7 +4674,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
+      <c r="N22" s="142"/>
       <c r="O22" s="8" t="s">
         <v>195</v>
       </c>
@@ -4722,7 +4725,7 @@
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
+      <c r="N23" s="142"/>
       <c r="O23" s="8" t="s">
         <v>195</v>
       </c>
@@ -4773,7 +4776,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
+      <c r="N24" s="142"/>
       <c r="O24" s="8" t="s">
         <v>195</v>
       </c>
@@ -4824,7 +4827,7 @@
       <c r="K25" s="107"/>
       <c r="L25" s="107"/>
       <c r="M25" s="107"/>
-      <c r="N25" s="107"/>
+      <c r="N25" s="142"/>
       <c r="O25" s="106" t="s">
         <v>195</v>
       </c>
@@ -4875,7 +4878,7 @@
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
+      <c r="N26" s="142"/>
       <c r="O26" s="8" t="s">
         <v>195</v>
       </c>
@@ -4926,7 +4929,7 @@
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
+      <c r="N27" s="142"/>
       <c r="O27" s="8" t="s">
         <v>195</v>
       </c>
@@ -4977,7 +4980,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
+      <c r="N28" s="142"/>
       <c r="O28" s="8" t="s">
         <v>195</v>
       </c>
@@ -5028,7 +5031,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
+      <c r="N29" s="142"/>
       <c r="O29" s="8" t="s">
         <v>195</v>
       </c>
@@ -5079,7 +5082,7 @@
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
+      <c r="N30" s="142"/>
       <c r="O30" s="8" t="s">
         <v>195</v>
       </c>
@@ -5130,7 +5133,7 @@
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
+      <c r="N31" s="142"/>
       <c r="O31" s="8" t="s">
         <v>195</v>
       </c>
@@ -5181,7 +5184,7 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
+      <c r="N32" s="142"/>
       <c r="O32" s="8" t="s">
         <v>195</v>
       </c>
@@ -5232,7 +5235,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
+      <c r="N33" s="142"/>
       <c r="O33" s="8" t="s">
         <v>195</v>
       </c>
@@ -5283,7 +5286,7 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
+      <c r="N34" s="142"/>
       <c r="O34" s="8" t="s">
         <v>195</v>
       </c>
@@ -5334,7 +5337,7 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
+      <c r="N35" s="142"/>
       <c r="O35" s="8" t="s">
         <v>195</v>
       </c>
@@ -5385,7 +5388,7 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
+      <c r="N36" s="142"/>
       <c r="O36" s="8" t="s">
         <v>195</v>
       </c>
@@ -5436,7 +5439,7 @@
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
+      <c r="N37" s="142"/>
       <c r="O37" s="8" t="s">
         <v>195</v>
       </c>
@@ -5487,7 +5490,7 @@
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
       <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
+      <c r="N38" s="142"/>
       <c r="O38" s="8" t="s">
         <v>195</v>
       </c>
@@ -5538,7 +5541,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
+      <c r="N39" s="142"/>
       <c r="O39" s="8" t="s">
         <v>195</v>
       </c>
@@ -5589,7 +5592,7 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
+      <c r="N40" s="142"/>
       <c r="O40" s="8" t="s">
         <v>195</v>
       </c>
@@ -5640,7 +5643,7 @@
       <c r="K41" s="7"/>
       <c r="L41" s="7"/>
       <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
+      <c r="N41" s="142"/>
       <c r="O41" s="8" t="s">
         <v>195</v>
       </c>
@@ -5691,7 +5694,7 @@
       <c r="K42" s="7"/>
       <c r="L42" s="7"/>
       <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
+      <c r="N42" s="142"/>
       <c r="O42" s="8" t="s">
         <v>195</v>
       </c>
@@ -5744,7 +5747,7 @@
         <v>401</v>
       </c>
       <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
+      <c r="N43" s="142"/>
       <c r="O43" s="8" t="s">
         <v>195</v>
       </c>
@@ -5796,7 +5799,7 @@
       <c r="M44" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="N44" s="7"/>
+      <c r="N44" s="142"/>
       <c r="O44" s="8" t="s">
         <v>195</v>
       </c>
@@ -7451,7 +7454,7 @@
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7462,7 +7465,7 @@
     <col min="4" max="4" width="16.5" style="40" customWidth="1"/>
     <col min="5" max="5" width="26.83203125" style="40" customWidth="1"/>
     <col min="6" max="11" width="14.5" style="40" customWidth="1"/>
-    <col min="12" max="251" width="8.83203125" customWidth="1"/>
+    <col min="12" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7798,7 +7801,7 @@
         <v>397</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E15" t="s">
         <v>271</v>
@@ -9157,8 +9160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C10"/>
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9835,7 +9838,7 @@
   <dimension ref="A1:IV50"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10217,277 +10220,277 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="8" t="s">
+    <row r="12" spans="1:256" s="144" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="136">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="136"/>
+      <c r="C12" s="137" t="s">
         <v>397</v>
       </c>
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="138" t="s">
+        <v>479</v>
+      </c>
+      <c r="E12" s="138" t="s">
         <v>480</v>
       </c>
-      <c r="E12" s="57" t="s">
-        <v>482</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="142"/>
+      <c r="G12" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="138" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="8" t="s">
+      <c r="I12" s="142"/>
+      <c r="J12" s="137" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="42"/>
-      <c r="V12" s="42"/>
-      <c r="W12" s="42"/>
-      <c r="X12" s="42"/>
-      <c r="Y12" s="42"/>
-      <c r="Z12" s="42"/>
-      <c r="AA12" s="42"/>
-      <c r="AB12" s="42"/>
-      <c r="AC12" s="42"/>
-      <c r="AD12" s="42"/>
-      <c r="AE12" s="42"/>
-      <c r="AF12" s="42"/>
-      <c r="AG12" s="42"/>
-      <c r="AH12" s="42"/>
-      <c r="AI12" s="42"/>
-      <c r="AJ12" s="42"/>
-      <c r="AK12" s="42"/>
-      <c r="AL12" s="42"/>
-      <c r="AM12" s="42"/>
-      <c r="AN12" s="42"/>
-      <c r="AO12" s="42"/>
-      <c r="AP12" s="42"/>
-      <c r="AQ12" s="42"/>
-      <c r="AR12" s="42"/>
-      <c r="AS12" s="42"/>
-      <c r="AT12" s="42"/>
-      <c r="AU12" s="42"/>
-      <c r="AV12" s="42"/>
-      <c r="AW12" s="42"/>
-      <c r="AX12" s="42"/>
-      <c r="AY12" s="42"/>
-      <c r="AZ12" s="42"/>
-      <c r="BA12" s="42"/>
-      <c r="BB12" s="42"/>
-      <c r="BC12" s="42"/>
-      <c r="BD12" s="42"/>
-      <c r="BE12" s="42"/>
-      <c r="BF12" s="42"/>
-      <c r="BG12" s="42"/>
-      <c r="BH12" s="42"/>
-      <c r="BI12" s="42"/>
-      <c r="BJ12" s="42"/>
-      <c r="BK12" s="42"/>
-      <c r="BL12" s="42"/>
-      <c r="BM12" s="42"/>
-      <c r="BN12" s="42"/>
-      <c r="BO12" s="42"/>
-      <c r="BP12" s="42"/>
-      <c r="BQ12" s="42"/>
-      <c r="BR12" s="42"/>
-      <c r="BS12" s="42"/>
-      <c r="BT12" s="42"/>
-      <c r="BU12" s="42"/>
-      <c r="BV12" s="42"/>
-      <c r="BW12" s="42"/>
-      <c r="BX12" s="42"/>
-      <c r="BY12" s="42"/>
-      <c r="BZ12" s="42"/>
-      <c r="CA12" s="42"/>
-      <c r="CB12" s="42"/>
-      <c r="CC12" s="42"/>
-      <c r="CD12" s="42"/>
-      <c r="CE12" s="42"/>
-      <c r="CF12" s="42"/>
-      <c r="CG12" s="42"/>
-      <c r="CH12" s="42"/>
-      <c r="CI12" s="42"/>
-      <c r="CJ12" s="42"/>
-      <c r="CK12" s="42"/>
-      <c r="CL12" s="42"/>
-      <c r="CM12" s="42"/>
-      <c r="CN12" s="42"/>
-      <c r="CO12" s="42"/>
-      <c r="CP12" s="42"/>
-      <c r="CQ12" s="42"/>
-      <c r="CR12" s="42"/>
-      <c r="CS12" s="42"/>
-      <c r="CT12" s="42"/>
-      <c r="CU12" s="42"/>
-      <c r="CV12" s="42"/>
-      <c r="CW12" s="42"/>
-      <c r="CX12" s="42"/>
-      <c r="CY12" s="42"/>
-      <c r="CZ12" s="42"/>
-      <c r="DA12" s="42"/>
-      <c r="DB12" s="42"/>
-      <c r="DC12" s="42"/>
-      <c r="DD12" s="42"/>
-      <c r="DE12" s="42"/>
-      <c r="DF12" s="42"/>
-      <c r="DG12" s="42"/>
-      <c r="DH12" s="42"/>
-      <c r="DI12" s="42"/>
-      <c r="DJ12" s="42"/>
-      <c r="DK12" s="42"/>
-      <c r="DL12" s="42"/>
-      <c r="DM12" s="42"/>
-      <c r="DN12" s="42"/>
-      <c r="DO12" s="42"/>
-      <c r="DP12" s="42"/>
-      <c r="DQ12" s="42"/>
-      <c r="DR12" s="42"/>
-      <c r="DS12" s="42"/>
-      <c r="DT12" s="42"/>
-      <c r="DU12" s="42"/>
-      <c r="DV12" s="42"/>
-      <c r="DW12" s="42"/>
-      <c r="DX12" s="42"/>
-      <c r="DY12" s="42"/>
-      <c r="DZ12" s="42"/>
-      <c r="EA12" s="42"/>
-      <c r="EB12" s="42"/>
-      <c r="EC12" s="42"/>
-      <c r="ED12" s="42"/>
-      <c r="EE12" s="42"/>
-      <c r="EF12" s="42"/>
-      <c r="EG12" s="42"/>
-      <c r="EH12" s="42"/>
-      <c r="EI12" s="42"/>
-      <c r="EJ12" s="42"/>
-      <c r="EK12" s="42"/>
-      <c r="EL12" s="42"/>
-      <c r="EM12" s="42"/>
-      <c r="EN12" s="42"/>
-      <c r="EO12" s="42"/>
-      <c r="EP12" s="42"/>
-      <c r="EQ12" s="42"/>
-      <c r="ER12" s="42"/>
-      <c r="ES12" s="42"/>
-      <c r="ET12" s="42"/>
-      <c r="EU12" s="42"/>
-      <c r="EV12" s="42"/>
-      <c r="EW12" s="42"/>
-      <c r="EX12" s="42"/>
-      <c r="EY12" s="42"/>
-      <c r="EZ12" s="42"/>
-      <c r="FA12" s="42"/>
-      <c r="FB12" s="42"/>
-      <c r="FC12" s="42"/>
-      <c r="FD12" s="42"/>
-      <c r="FE12" s="42"/>
-      <c r="FF12" s="42"/>
-      <c r="FG12" s="42"/>
-      <c r="FH12" s="42"/>
-      <c r="FI12" s="42"/>
-      <c r="FJ12" s="42"/>
-      <c r="FK12" s="42"/>
-      <c r="FL12" s="42"/>
-      <c r="FM12" s="42"/>
-      <c r="FN12" s="42"/>
-      <c r="FO12" s="42"/>
-      <c r="FP12" s="42"/>
-      <c r="FQ12" s="42"/>
-      <c r="FR12" s="42"/>
-      <c r="FS12" s="42"/>
-      <c r="FT12" s="42"/>
-      <c r="FU12" s="42"/>
-      <c r="FV12" s="42"/>
-      <c r="FW12" s="42"/>
-      <c r="FX12" s="42"/>
-      <c r="FY12" s="42"/>
-      <c r="FZ12" s="42"/>
-      <c r="GA12" s="42"/>
-      <c r="GB12" s="42"/>
-      <c r="GC12" s="42"/>
-      <c r="GD12" s="42"/>
-      <c r="GE12" s="42"/>
-      <c r="GF12" s="42"/>
-      <c r="GG12" s="42"/>
-      <c r="GH12" s="42"/>
-      <c r="GI12" s="42"/>
-      <c r="GJ12" s="42"/>
-      <c r="GK12" s="42"/>
-      <c r="GL12" s="42"/>
-      <c r="GM12" s="42"/>
-      <c r="GN12" s="42"/>
-      <c r="GO12" s="42"/>
-      <c r="GP12" s="42"/>
-      <c r="GQ12" s="42"/>
-      <c r="GR12" s="42"/>
-      <c r="GS12" s="42"/>
-      <c r="GT12" s="42"/>
-      <c r="GU12" s="42"/>
-      <c r="GV12" s="42"/>
-      <c r="GW12" s="42"/>
-      <c r="GX12" s="42"/>
-      <c r="GY12" s="42"/>
-      <c r="GZ12" s="42"/>
-      <c r="HA12" s="42"/>
-      <c r="HB12" s="42"/>
-      <c r="HC12" s="42"/>
-      <c r="HD12" s="42"/>
-      <c r="HE12" s="42"/>
-      <c r="HF12" s="42"/>
-      <c r="HG12" s="42"/>
-      <c r="HH12" s="42"/>
-      <c r="HI12" s="42"/>
-      <c r="HJ12" s="42"/>
-      <c r="HK12" s="42"/>
-      <c r="HL12" s="42"/>
-      <c r="HM12" s="42"/>
-      <c r="HN12" s="42"/>
-      <c r="HO12" s="42"/>
-      <c r="HP12" s="42"/>
-      <c r="HQ12" s="42"/>
-      <c r="HR12" s="42"/>
-      <c r="HS12" s="42"/>
-      <c r="HT12" s="42"/>
-      <c r="HU12" s="42"/>
-      <c r="HV12" s="42"/>
-      <c r="HW12" s="42"/>
-      <c r="HX12" s="42"/>
-      <c r="HY12" s="42"/>
-      <c r="HZ12" s="42"/>
-      <c r="IA12" s="42"/>
-      <c r="IB12" s="42"/>
-      <c r="IC12" s="42"/>
-      <c r="ID12" s="42"/>
-      <c r="IE12" s="42"/>
-      <c r="IF12" s="42"/>
-      <c r="IG12" s="42"/>
-      <c r="IH12" s="42"/>
-      <c r="II12" s="42"/>
-      <c r="IJ12" s="42"/>
-      <c r="IK12" s="42"/>
-      <c r="IL12" s="42"/>
-      <c r="IM12" s="42"/>
-      <c r="IN12" s="42"/>
-      <c r="IO12" s="42"/>
-      <c r="IP12" s="42"/>
-      <c r="IQ12" s="42"/>
-      <c r="IR12" s="42"/>
-      <c r="IS12" s="42"/>
-      <c r="IT12" s="42"/>
-      <c r="IU12" s="42"/>
-      <c r="IV12" s="42"/>
+      <c r="K12" s="142"/>
+      <c r="L12" s="142"/>
+      <c r="M12" s="142"/>
+      <c r="N12" s="142"/>
+      <c r="O12" s="142"/>
+      <c r="P12" s="142"/>
+      <c r="Q12" s="142"/>
+      <c r="R12" s="145"/>
+      <c r="S12" s="145"/>
+      <c r="T12" s="145"/>
+      <c r="U12" s="145"/>
+      <c r="V12" s="145"/>
+      <c r="W12" s="145"/>
+      <c r="X12" s="145"/>
+      <c r="Y12" s="145"/>
+      <c r="Z12" s="145"/>
+      <c r="AA12" s="145"/>
+      <c r="AB12" s="145"/>
+      <c r="AC12" s="145"/>
+      <c r="AD12" s="145"/>
+      <c r="AE12" s="145"/>
+      <c r="AF12" s="145"/>
+      <c r="AG12" s="145"/>
+      <c r="AH12" s="145"/>
+      <c r="AI12" s="145"/>
+      <c r="AJ12" s="145"/>
+      <c r="AK12" s="145"/>
+      <c r="AL12" s="145"/>
+      <c r="AM12" s="145"/>
+      <c r="AN12" s="145"/>
+      <c r="AO12" s="145"/>
+      <c r="AP12" s="145"/>
+      <c r="AQ12" s="145"/>
+      <c r="AR12" s="145"/>
+      <c r="AS12" s="145"/>
+      <c r="AT12" s="145"/>
+      <c r="AU12" s="145"/>
+      <c r="AV12" s="145"/>
+      <c r="AW12" s="145"/>
+      <c r="AX12" s="145"/>
+      <c r="AY12" s="145"/>
+      <c r="AZ12" s="145"/>
+      <c r="BA12" s="145"/>
+      <c r="BB12" s="145"/>
+      <c r="BC12" s="145"/>
+      <c r="BD12" s="145"/>
+      <c r="BE12" s="145"/>
+      <c r="BF12" s="145"/>
+      <c r="BG12" s="145"/>
+      <c r="BH12" s="145"/>
+      <c r="BI12" s="145"/>
+      <c r="BJ12" s="145"/>
+      <c r="BK12" s="145"/>
+      <c r="BL12" s="145"/>
+      <c r="BM12" s="145"/>
+      <c r="BN12" s="145"/>
+      <c r="BO12" s="145"/>
+      <c r="BP12" s="145"/>
+      <c r="BQ12" s="145"/>
+      <c r="BR12" s="145"/>
+      <c r="BS12" s="145"/>
+      <c r="BT12" s="145"/>
+      <c r="BU12" s="145"/>
+      <c r="BV12" s="145"/>
+      <c r="BW12" s="145"/>
+      <c r="BX12" s="145"/>
+      <c r="BY12" s="145"/>
+      <c r="BZ12" s="145"/>
+      <c r="CA12" s="145"/>
+      <c r="CB12" s="145"/>
+      <c r="CC12" s="145"/>
+      <c r="CD12" s="145"/>
+      <c r="CE12" s="145"/>
+      <c r="CF12" s="145"/>
+      <c r="CG12" s="145"/>
+      <c r="CH12" s="145"/>
+      <c r="CI12" s="145"/>
+      <c r="CJ12" s="145"/>
+      <c r="CK12" s="145"/>
+      <c r="CL12" s="145"/>
+      <c r="CM12" s="145"/>
+      <c r="CN12" s="145"/>
+      <c r="CO12" s="145"/>
+      <c r="CP12" s="145"/>
+      <c r="CQ12" s="145"/>
+      <c r="CR12" s="145"/>
+      <c r="CS12" s="145"/>
+      <c r="CT12" s="145"/>
+      <c r="CU12" s="145"/>
+      <c r="CV12" s="145"/>
+      <c r="CW12" s="145"/>
+      <c r="CX12" s="145"/>
+      <c r="CY12" s="145"/>
+      <c r="CZ12" s="145"/>
+      <c r="DA12" s="145"/>
+      <c r="DB12" s="145"/>
+      <c r="DC12" s="145"/>
+      <c r="DD12" s="145"/>
+      <c r="DE12" s="145"/>
+      <c r="DF12" s="145"/>
+      <c r="DG12" s="145"/>
+      <c r="DH12" s="145"/>
+      <c r="DI12" s="145"/>
+      <c r="DJ12" s="145"/>
+      <c r="DK12" s="145"/>
+      <c r="DL12" s="145"/>
+      <c r="DM12" s="145"/>
+      <c r="DN12" s="145"/>
+      <c r="DO12" s="145"/>
+      <c r="DP12" s="145"/>
+      <c r="DQ12" s="145"/>
+      <c r="DR12" s="145"/>
+      <c r="DS12" s="145"/>
+      <c r="DT12" s="145"/>
+      <c r="DU12" s="145"/>
+      <c r="DV12" s="145"/>
+      <c r="DW12" s="145"/>
+      <c r="DX12" s="145"/>
+      <c r="DY12" s="145"/>
+      <c r="DZ12" s="145"/>
+      <c r="EA12" s="145"/>
+      <c r="EB12" s="145"/>
+      <c r="EC12" s="145"/>
+      <c r="ED12" s="145"/>
+      <c r="EE12" s="145"/>
+      <c r="EF12" s="145"/>
+      <c r="EG12" s="145"/>
+      <c r="EH12" s="145"/>
+      <c r="EI12" s="145"/>
+      <c r="EJ12" s="145"/>
+      <c r="EK12" s="145"/>
+      <c r="EL12" s="145"/>
+      <c r="EM12" s="145"/>
+      <c r="EN12" s="145"/>
+      <c r="EO12" s="145"/>
+      <c r="EP12" s="145"/>
+      <c r="EQ12" s="145"/>
+      <c r="ER12" s="145"/>
+      <c r="ES12" s="145"/>
+      <c r="ET12" s="145"/>
+      <c r="EU12" s="145"/>
+      <c r="EV12" s="145"/>
+      <c r="EW12" s="145"/>
+      <c r="EX12" s="145"/>
+      <c r="EY12" s="145"/>
+      <c r="EZ12" s="145"/>
+      <c r="FA12" s="145"/>
+      <c r="FB12" s="145"/>
+      <c r="FC12" s="145"/>
+      <c r="FD12" s="145"/>
+      <c r="FE12" s="145"/>
+      <c r="FF12" s="145"/>
+      <c r="FG12" s="145"/>
+      <c r="FH12" s="145"/>
+      <c r="FI12" s="145"/>
+      <c r="FJ12" s="145"/>
+      <c r="FK12" s="145"/>
+      <c r="FL12" s="145"/>
+      <c r="FM12" s="145"/>
+      <c r="FN12" s="145"/>
+      <c r="FO12" s="145"/>
+      <c r="FP12" s="145"/>
+      <c r="FQ12" s="145"/>
+      <c r="FR12" s="145"/>
+      <c r="FS12" s="145"/>
+      <c r="FT12" s="145"/>
+      <c r="FU12" s="145"/>
+      <c r="FV12" s="145"/>
+      <c r="FW12" s="145"/>
+      <c r="FX12" s="145"/>
+      <c r="FY12" s="145"/>
+      <c r="FZ12" s="145"/>
+      <c r="GA12" s="145"/>
+      <c r="GB12" s="145"/>
+      <c r="GC12" s="145"/>
+      <c r="GD12" s="145"/>
+      <c r="GE12" s="145"/>
+      <c r="GF12" s="145"/>
+      <c r="GG12" s="145"/>
+      <c r="GH12" s="145"/>
+      <c r="GI12" s="145"/>
+      <c r="GJ12" s="145"/>
+      <c r="GK12" s="145"/>
+      <c r="GL12" s="145"/>
+      <c r="GM12" s="145"/>
+      <c r="GN12" s="145"/>
+      <c r="GO12" s="145"/>
+      <c r="GP12" s="145"/>
+      <c r="GQ12" s="145"/>
+      <c r="GR12" s="145"/>
+      <c r="GS12" s="145"/>
+      <c r="GT12" s="145"/>
+      <c r="GU12" s="145"/>
+      <c r="GV12" s="145"/>
+      <c r="GW12" s="145"/>
+      <c r="GX12" s="145"/>
+      <c r="GY12" s="145"/>
+      <c r="GZ12" s="145"/>
+      <c r="HA12" s="145"/>
+      <c r="HB12" s="145"/>
+      <c r="HC12" s="145"/>
+      <c r="HD12" s="145"/>
+      <c r="HE12" s="145"/>
+      <c r="HF12" s="145"/>
+      <c r="HG12" s="145"/>
+      <c r="HH12" s="145"/>
+      <c r="HI12" s="145"/>
+      <c r="HJ12" s="145"/>
+      <c r="HK12" s="145"/>
+      <c r="HL12" s="145"/>
+      <c r="HM12" s="145"/>
+      <c r="HN12" s="145"/>
+      <c r="HO12" s="145"/>
+      <c r="HP12" s="145"/>
+      <c r="HQ12" s="145"/>
+      <c r="HR12" s="145"/>
+      <c r="HS12" s="145"/>
+      <c r="HT12" s="145"/>
+      <c r="HU12" s="145"/>
+      <c r="HV12" s="145"/>
+      <c r="HW12" s="145"/>
+      <c r="HX12" s="145"/>
+      <c r="HY12" s="145"/>
+      <c r="HZ12" s="145"/>
+      <c r="IA12" s="145"/>
+      <c r="IB12" s="145"/>
+      <c r="IC12" s="145"/>
+      <c r="ID12" s="145"/>
+      <c r="IE12" s="145"/>
+      <c r="IF12" s="145"/>
+      <c r="IG12" s="145"/>
+      <c r="IH12" s="145"/>
+      <c r="II12" s="145"/>
+      <c r="IJ12" s="145"/>
+      <c r="IK12" s="145"/>
+      <c r="IL12" s="145"/>
+      <c r="IM12" s="145"/>
+      <c r="IN12" s="145"/>
+      <c r="IO12" s="145"/>
+      <c r="IP12" s="145"/>
+      <c r="IQ12" s="145"/>
+      <c r="IR12" s="145"/>
+      <c r="IS12" s="145"/>
+      <c r="IT12" s="145"/>
+      <c r="IU12" s="145"/>
+      <c r="IV12" s="145"/>
     </row>
     <row r="13" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10">
@@ -19818,7 +19821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="K4" sqref="K4:K7"/>
     </sheetView>
   </sheetViews>
@@ -21038,8 +21041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E561A8A-480D-6D45-8F14-5D4A9428A511}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G4:G7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21168,7 +21171,6 @@
       <c r="F4" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="84"/>
       <c r="I4">
         <v>1</v>
       </c>
@@ -21192,7 +21194,6 @@
       <c r="F5" s="84" t="s">
         <v>446</v>
       </c>
-      <c r="G5" s="84"/>
       <c r="I5">
         <v>2</v>
       </c>
@@ -21216,7 +21217,6 @@
       <c r="F6" s="84" t="s">
         <v>463</v>
       </c>
-      <c r="G6" s="84"/>
       <c r="I6">
         <v>1</v>
       </c>
@@ -21240,7 +21240,6 @@
       <c r="F7" s="84" t="s">
         <v>464</v>
       </c>
-      <c r="G7" s="84"/>
       <c r="I7">
         <v>7</v>
       </c>
@@ -21296,7 +21295,6 @@
       <c r="F9" s="84" t="s">
         <v>467</v>
       </c>
-      <c r="G9" s="84"/>
       <c r="I9">
         <v>6</v>
       </c>
@@ -21320,7 +21318,6 @@
       <c r="F10" s="84" t="s">
         <v>468</v>
       </c>
-      <c r="G10" s="84"/>
       <c r="I10">
         <v>5</v>
       </c>
@@ -21344,7 +21341,6 @@
       <c r="F11" s="84" t="s">
         <v>469</v>
       </c>
-      <c r="G11" s="84"/>
       <c r="I11">
         <v>8</v>
       </c>
@@ -21371,7 +21367,6 @@
       <c r="F12" s="84" t="s">
         <v>465</v>
       </c>
-      <c r="G12" s="84"/>
       <c r="J12" s="84" t="s">
         <v>438</v>
       </c>
@@ -21718,10 +21713,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21736,7 +21731,8 @@
     <col min="9" max="9" width="21" style="18" customWidth="1"/>
     <col min="10" max="10" width="30.33203125" style="18" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" style="18" customWidth="1"/>
-    <col min="12" max="14" width="8.83203125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="145" customWidth="1"/>
+    <col min="13" max="14" width="8.83203125" style="18" customWidth="1"/>
     <col min="15" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -21760,7 +21756,7 @@
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="L1" s="142"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
     </row>
@@ -21798,11 +21794,11 @@
       <c r="K2" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="L2" s="7"/>
+      <c r="L2" s="142"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -21836,45 +21832,45 @@
       <c r="K3" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="L3" s="137" t="s">
-        <v>479</v>
+      <c r="L3" s="147" t="s">
+        <v>483</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="8" t="s">
+    <row r="4" spans="1:14" s="144" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="136">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="136"/>
+      <c r="C4" s="137" t="s">
         <v>397</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="137" t="s">
         <v>157</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="138" t="s">
         <v>155</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="G4" s="134">
+      <c r="G4" s="140">
         <v>2</v>
       </c>
-      <c r="H4" s="57" t="s">
-        <v>480</v>
-      </c>
-      <c r="I4" s="6">
+      <c r="H4" s="138" t="s">
+        <v>479</v>
+      </c>
+      <c r="I4" s="141">
         <v>2</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="138" t="s">
-        <v>483</v>
-      </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="143" t="s">
+        <v>481</v>
+      </c>
+      <c r="M4" s="142"/>
+      <c r="N4" s="142"/>
     </row>
     <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
@@ -21904,7 +21900,7 @@
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="L5" s="142"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
     </row>
@@ -21936,41 +21932,41 @@
       </c>
       <c r="J6" s="116"/>
       <c r="K6" s="116"/>
-      <c r="L6" s="116"/>
+      <c r="L6" s="142"/>
       <c r="M6" s="116"/>
       <c r="N6" s="116"/>
     </row>
-    <row r="7" spans="1:14" s="93" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="111">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="112" t="s">
-        <v>397</v>
-      </c>
-      <c r="D7" s="112" t="s">
+    <row r="7" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>155</v>
+      <c r="E7" s="57" t="s">
+        <v>156</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>156</v>
       </c>
       <c r="G7" s="135">
-        <v>1</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I7" s="115">
-        <v>1</v>
-      </c>
-      <c r="J7" s="116"/>
-      <c r="K7" s="116"/>
-      <c r="L7" s="138"/>
-      <c r="M7" s="116"/>
-      <c r="N7" s="116"/>
+        <v>2</v>
+      </c>
+      <c r="H7" s="57" t="s">
+        <v>367</v>
+      </c>
+      <c r="I7" s="6">
+        <v>2</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="142"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
@@ -21992,113 +21988,113 @@
       <c r="G8" s="135">
         <v>2</v>
       </c>
-      <c r="H8" s="57" t="s">
-        <v>367</v>
+      <c r="H8" s="8" t="s">
+        <v>276</v>
       </c>
       <c r="I8" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="L8" s="142"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="8" t="s">
+    <row r="9" spans="1:14" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="111">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="111"/>
+      <c r="C9" s="112" t="s">
         <v>275</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="E9" s="57" t="s">
-        <v>156</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>156</v>
+      <c r="E9" s="113" t="s">
+        <v>476</v>
+      </c>
+      <c r="F9" s="114" t="s">
+        <v>476</v>
       </c>
       <c r="G9" s="135">
-        <v>2</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="I9" s="6">
         <v>1</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-    </row>
-    <row r="10" spans="1:14" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="111">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="111"/>
-      <c r="C10" s="112" t="s">
-        <v>275</v>
-      </c>
-      <c r="D10" s="112" t="s">
+      <c r="H9" s="112" t="s">
+        <v>475</v>
+      </c>
+      <c r="I9" s="115">
+        <v>1</v>
+      </c>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="142"/>
+      <c r="M9" s="116"/>
+      <c r="N9" s="116"/>
+    </row>
+    <row r="10" spans="1:14" s="133" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="127">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="127"/>
+      <c r="C10" s="128" t="s">
+        <v>330</v>
+      </c>
+      <c r="D10" s="129" t="s">
         <v>157</v>
       </c>
-      <c r="E10" s="113" t="s">
+      <c r="E10" s="128" t="s">
         <v>476</v>
       </c>
-      <c r="F10" s="114" t="s">
+      <c r="F10" s="130" t="s">
         <v>476</v>
       </c>
       <c r="G10" s="135">
         <v>1</v>
       </c>
-      <c r="H10" s="112" t="s">
+      <c r="H10" s="129" t="s">
         <v>475</v>
       </c>
-      <c r="I10" s="115">
+      <c r="I10" s="131">
         <v>1</v>
       </c>
-      <c r="J10" s="116"/>
-      <c r="K10" s="116"/>
-      <c r="L10" s="116"/>
-      <c r="M10" s="116"/>
-      <c r="N10" s="116"/>
-    </row>
-    <row r="11" spans="1:14" s="133" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="127">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="127"/>
-      <c r="C11" s="128" t="s">
+      <c r="J10" s="132"/>
+      <c r="K10" s="132"/>
+      <c r="L10" s="142"/>
+      <c r="M10" s="132"/>
+      <c r="N10" s="132"/>
+    </row>
+    <row r="11" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="57" t="s">
         <v>330</v>
       </c>
-      <c r="D11" s="129" t="s">
+      <c r="D11" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E11" s="128" t="s">
-        <v>476</v>
-      </c>
-      <c r="F11" s="130" t="s">
-        <v>476</v>
+      <c r="E11" s="57" t="s">
+        <v>323</v>
+      </c>
+      <c r="F11" s="57" t="s">
+        <v>323</v>
       </c>
       <c r="G11" s="135">
-        <v>1</v>
-      </c>
-      <c r="H11" s="129" t="s">
-        <v>475</v>
-      </c>
-      <c r="I11" s="131">
-        <v>1</v>
-      </c>
-      <c r="J11" s="132"/>
-      <c r="K11" s="132"/>
-      <c r="L11" s="132"/>
-      <c r="M11" s="132"/>
-      <c r="N11" s="132"/>
+        <v>3</v>
+      </c>
+      <c r="H11" s="57" t="s">
+        <v>335</v>
+      </c>
+      <c r="I11" s="6">
+        <v>3</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="142"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
     </row>
     <row r="12" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10">
@@ -22121,14 +22117,14 @@
         <v>3</v>
       </c>
       <c r="H12" s="57" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="I12" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
+      <c r="L12" s="142"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
     </row>
@@ -22153,14 +22149,14 @@
         <v>3</v>
       </c>
       <c r="H13" s="57" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="I13" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
+      <c r="L13" s="142"/>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
     </row>
@@ -22176,23 +22172,23 @@
         <v>157</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F14" s="57" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G14" s="135">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I14" s="6">
         <v>1</v>
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="L14" s="142"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
     </row>
@@ -22208,23 +22204,23 @@
         <v>157</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F15" s="57" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G15" s="135">
-        <v>2</v>
-      </c>
-      <c r="H15" s="57" t="s">
-        <v>333</v>
+        <v>4</v>
+      </c>
+      <c r="H15" s="59" t="s">
+        <v>365</v>
       </c>
       <c r="I15" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="142"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
     </row>
@@ -22248,15 +22244,15 @@
       <c r="G16" s="135">
         <v>4</v>
       </c>
-      <c r="H16" s="59" t="s">
-        <v>365</v>
+      <c r="H16" s="63" t="s">
+        <v>349</v>
       </c>
       <c r="I16" s="6">
         <v>3</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="65"/>
-      <c r="L16" s="7"/>
+      <c r="L16" s="142"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
     </row>
@@ -22281,14 +22277,14 @@
         <v>4</v>
       </c>
       <c r="H17" s="63" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="I17" s="6">
         <v>3</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="65"/>
-      <c r="L17" s="7"/>
+      <c r="L17" s="142"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
     </row>
@@ -22304,23 +22300,25 @@
         <v>157</v>
       </c>
       <c r="E18" s="57" t="s">
-        <v>324</v>
+        <v>362</v>
       </c>
       <c r="F18" s="57" t="s">
-        <v>324</v>
+        <v>359</v>
       </c>
       <c r="G18" s="135">
-        <v>4</v>
-      </c>
-      <c r="H18" s="63" t="s">
-        <v>355</v>
+        <v>5</v>
+      </c>
+      <c r="H18" s="57" t="s">
+        <v>336</v>
       </c>
       <c r="I18" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J18" s="7"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="7"/>
+      <c r="K18" s="59" t="s">
+        <v>371</v>
+      </c>
+      <c r="L18" s="142"/>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
     </row>
@@ -22336,25 +22334,25 @@
         <v>157</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F19" s="57" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G19" s="135">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H19" s="57" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="I19" s="6">
         <v>1</v>
       </c>
       <c r="J19" s="7"/>
-      <c r="K19" s="59" t="s">
-        <v>371</v>
-      </c>
-      <c r="L19" s="7"/>
+      <c r="K19" s="63" t="s">
+        <v>373</v>
+      </c>
+      <c r="L19" s="142"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
     </row>
@@ -22370,59 +22368,57 @@
         <v>157</v>
       </c>
       <c r="E20" s="57" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F20" s="57" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G20" s="135">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H20" s="57" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="I20" s="6">
         <v>1</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="63" t="s">
-        <v>373</v>
-      </c>
-      <c r="L20" s="7"/>
+        <v>372</v>
+      </c>
+      <c r="L20" s="142"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>42736</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="57" t="s">
-        <v>330</v>
+      <c r="C21" s="8" t="s">
+        <v>285</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E21" s="57" t="s">
-        <v>364</v>
-      </c>
-      <c r="F21" s="57" t="s">
-        <v>361</v>
+      <c r="E21" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>312</v>
       </c>
       <c r="G21" s="135">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H21" s="57" t="s">
-        <v>339</v>
+        <v>311</v>
       </c>
       <c r="I21" s="6">
         <v>1</v>
       </c>
       <c r="J21" s="7"/>
-      <c r="K21" s="63" t="s">
-        <v>372</v>
-      </c>
-      <c r="L21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="142"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
     </row>
@@ -22437,90 +22433,90 @@
       <c r="D22" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>313</v>
+      <c r="E22" s="57" t="s">
+        <v>443</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>312</v>
+        <v>457</v>
       </c>
       <c r="G22" s="135">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H22" s="57" t="s">
-        <v>311</v>
+        <v>455</v>
       </c>
       <c r="I22" s="6">
         <v>1</v>
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
+      <c r="L22" s="142"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="8" t="s">
+    <row r="23" spans="1:14" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="111">
+        <v>42736</v>
+      </c>
+      <c r="B23" s="111"/>
+      <c r="C23" s="112" t="s">
         <v>285</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="57" t="s">
-        <v>443</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>457</v>
+      <c r="E23" s="113" t="s">
+        <v>476</v>
+      </c>
+      <c r="F23" s="114" t="s">
+        <v>476</v>
       </c>
       <c r="G23" s="135">
-        <v>3</v>
-      </c>
-      <c r="H23" s="57" t="s">
-        <v>455</v>
-      </c>
-      <c r="I23" s="6">
         <v>1</v>
       </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-    </row>
-    <row r="24" spans="1:14" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="111">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="111"/>
-      <c r="C24" s="112" t="s">
-        <v>285</v>
-      </c>
-      <c r="D24" s="112" t="s">
+      <c r="H23" s="112" t="s">
+        <v>475</v>
+      </c>
+      <c r="I23" s="115">
+        <v>1</v>
+      </c>
+      <c r="J23" s="116"/>
+      <c r="K23" s="116"/>
+      <c r="L23" s="142"/>
+      <c r="M23" s="116"/>
+      <c r="N23" s="116"/>
+    </row>
+    <row r="24" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E24" s="113" t="s">
-        <v>476</v>
-      </c>
-      <c r="F24" s="114" t="s">
-        <v>476</v>
+      <c r="E24" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>390</v>
       </c>
       <c r="G24" s="135">
+        <v>2</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I24" s="6">
         <v>1</v>
       </c>
-      <c r="H24" s="112" t="s">
-        <v>475</v>
-      </c>
-      <c r="I24" s="115">
-        <v>1</v>
-      </c>
-      <c r="J24" s="116"/>
-      <c r="K24" s="116"/>
-      <c r="L24" s="116"/>
-      <c r="M24" s="116"/>
-      <c r="N24" s="116"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="142"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
     </row>
     <row r="25" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
@@ -22543,14 +22539,14 @@
         <v>2</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>388</v>
+        <v>333</v>
       </c>
       <c r="I25" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
+      <c r="L25" s="142"/>
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
     </row>
@@ -22575,14 +22571,14 @@
         <v>2</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="I26" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
+      <c r="L26" s="142"/>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
     </row>
@@ -22607,144 +22603,146 @@
         <v>2</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="I27" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
+      <c r="L27" s="142"/>
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="8" t="s">
+    <row r="28" spans="1:14" s="133" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="127">
+        <v>42736</v>
+      </c>
+      <c r="B28" s="127"/>
+      <c r="C28" s="129" t="s">
         <v>374</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="129" t="s">
         <v>157</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>390</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>390</v>
-      </c>
-      <c r="G28" s="135">
+      <c r="E28" s="130" t="s">
+        <v>476</v>
+      </c>
+      <c r="F28" s="130" t="s">
+        <v>476</v>
+      </c>
+      <c r="G28" s="131">
+        <v>1</v>
+      </c>
+      <c r="H28" s="128" t="s">
+        <v>475</v>
+      </c>
+      <c r="I28" s="131">
+        <v>4</v>
+      </c>
+      <c r="J28" s="132"/>
+      <c r="K28" s="132"/>
+      <c r="L28" s="142"/>
+      <c r="M28" s="132"/>
+      <c r="N28" s="132"/>
+    </row>
+    <row r="29" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="G29" s="135">
         <v>2</v>
       </c>
-      <c r="H28" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="I28" s="6">
-        <v>4</v>
-      </c>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-    </row>
-    <row r="29" spans="1:14" s="133" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="127">
-        <v>42736</v>
-      </c>
-      <c r="B29" s="127"/>
-      <c r="C29" s="129" t="s">
-        <v>374</v>
-      </c>
-      <c r="D29" s="129" t="s">
+      <c r="H29" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I29" s="6">
+        <v>1</v>
+      </c>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="142"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+    </row>
+    <row r="30" spans="1:14" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="111">
+        <v>42736</v>
+      </c>
+      <c r="B30" s="111"/>
+      <c r="C30" s="112" t="s">
+        <v>393</v>
+      </c>
+      <c r="D30" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="E29" s="130" t="s">
+      <c r="E30" s="114" t="s">
         <v>476</v>
       </c>
-      <c r="F29" s="130" t="s">
+      <c r="F30" s="114" t="s">
         <v>476</v>
       </c>
-      <c r="G29" s="131">
+      <c r="G30" s="135">
         <v>1</v>
       </c>
-      <c r="H29" s="128" t="s">
+      <c r="H30" s="113" t="s">
         <v>475</v>
       </c>
-      <c r="I29" s="131">
-        <v>4</v>
-      </c>
-      <c r="J29" s="132"/>
-      <c r="K29" s="132"/>
-      <c r="L29" s="132"/>
-      <c r="M29" s="132"/>
-      <c r="N29" s="132"/>
-    </row>
-    <row r="30" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="D30" s="8" t="s">
+      <c r="I30" s="115">
+        <v>1</v>
+      </c>
+      <c r="J30" s="116"/>
+      <c r="K30" s="116"/>
+      <c r="L30" s="142"/>
+      <c r="M30" s="116"/>
+      <c r="N30" s="116"/>
+    </row>
+    <row r="31" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E30" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="G30" s="135">
+      <c r="E31" s="57" t="s">
+        <v>362</v>
+      </c>
+      <c r="F31" s="57" t="s">
+        <v>359</v>
+      </c>
+      <c r="G31" s="135">
         <v>2</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H31" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I31" s="6">
         <v>1</v>
       </c>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-    </row>
-    <row r="31" spans="1:14" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="111">
-        <v>42736</v>
-      </c>
-      <c r="B31" s="111"/>
-      <c r="C31" s="112" t="s">
-        <v>393</v>
-      </c>
-      <c r="D31" s="112" t="s">
-        <v>157</v>
-      </c>
-      <c r="E31" s="114" t="s">
-        <v>476</v>
-      </c>
-      <c r="F31" s="114" t="s">
-        <v>476</v>
-      </c>
-      <c r="G31" s="135">
-        <v>1</v>
-      </c>
-      <c r="H31" s="113" t="s">
-        <v>475</v>
-      </c>
-      <c r="I31" s="115">
-        <v>1</v>
-      </c>
-      <c r="J31" s="116"/>
-      <c r="K31" s="116"/>
-      <c r="L31" s="116"/>
-      <c r="M31" s="116"/>
-      <c r="N31" s="116"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="59" t="s">
+        <v>401</v>
+      </c>
+      <c r="L31" s="142"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
     </row>
     <row r="32" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10">
@@ -22767,85 +22765,52 @@
         <v>2</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>66</v>
+        <v>337</v>
       </c>
       <c r="I32" s="6">
         <v>1</v>
       </c>
-      <c r="J32" s="7"/>
-      <c r="K32" s="59" t="s">
-        <v>401</v>
-      </c>
-      <c r="L32" s="7"/>
+      <c r="J32" s="59" t="s">
+        <v>405</v>
+      </c>
+      <c r="K32" s="59"/>
+      <c r="L32" s="142"/>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
     </row>
-    <row r="33" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="8" t="s">
+    <row r="33" spans="1:14" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="87">
+        <v>42736</v>
+      </c>
+      <c r="B33" s="87"/>
+      <c r="C33" s="89" t="s">
         <v>398</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="E33" s="57" t="s">
-        <v>362</v>
-      </c>
-      <c r="F33" s="57" t="s">
-        <v>359</v>
+      <c r="E33" s="103" t="s">
+        <v>476</v>
+      </c>
+      <c r="F33" s="103" t="s">
+        <v>476</v>
       </c>
       <c r="G33" s="135">
-        <v>2</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="I33" s="6">
         <v>1</v>
       </c>
-      <c r="J33" s="59" t="s">
-        <v>405</v>
-      </c>
-      <c r="K33" s="59"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-    </row>
-    <row r="34" spans="1:14" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="87">
-        <v>42736</v>
-      </c>
-      <c r="B34" s="87"/>
-      <c r="C34" s="89" t="s">
-        <v>398</v>
-      </c>
-      <c r="D34" s="89" t="s">
-        <v>157</v>
-      </c>
-      <c r="E34" s="103" t="s">
-        <v>476</v>
-      </c>
-      <c r="F34" s="103" t="s">
-        <v>476</v>
-      </c>
-      <c r="G34" s="135">
+      <c r="H33" s="103" t="s">
+        <v>475</v>
+      </c>
+      <c r="I33" s="117">
         <v>1</v>
       </c>
-      <c r="H34" s="103" t="s">
-        <v>475</v>
-      </c>
-      <c r="I34" s="117">
-        <v>1</v>
-      </c>
-      <c r="J34" s="118"/>
-      <c r="K34" s="118"/>
-      <c r="L34" s="119"/>
-      <c r="M34" s="119"/>
-      <c r="N34" s="119"/>
-    </row>
+      <c r="J33" s="118"/>
+      <c r="K33" s="118"/>
+      <c r="L33" s="142"/>
+      <c r="M33" s="119"/>
+      <c r="N33" s="119"/>
+    </row>
+    <row r="36" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>